<commit_message>
Started export EXE for unittestcases
</commit_message>
<xml_diff>
--- a/test_sets_UpdateTracking.xlsx
+++ b/test_sets_UpdateTracking.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\0_Wissenschaftlicher Mitarbeiter\PhD\dev\Update_Tracking\test_sets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\hiwi\Beispiel_dateien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14AECF9-4639-4974-9C20-468018EAD990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21840" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{18A16E2F-57C6-4CB6-ACB7-BDD71A03C075}"/>
+    <workbookView xWindow="21840" yWindow="-105" windowWidth="33120" windowHeight="18120"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,8 +32,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Stefan</author>
+  </authors>
+  <commentList>
+    <comment ref="D5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Stefan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Was ist hier mit Subgraphs gemeint? 
+Einfach ein IfcProdukt?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
   <si>
     <t>Nr</t>
   </si>
@@ -216,13 +250,16 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +274,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -274,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -282,38 +332,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -321,16 +391,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -643,395 +703,441 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE5B51C0-91F9-4228-A7A4-16636B385B0B}">
-  <dimension ref="A2:I29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.84375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.3828125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.69140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="51.765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62" style="5" customWidth="1"/>
-    <col min="6" max="6" width="41.4609375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="11.765625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="25.07421875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.07421875" style="1"/>
+    <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62" style="4" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="11.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="9" t="s">
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J3" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-    </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="J6" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="E10" s="3"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H13" s="7"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H14" s="7"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="2:8" s="2" customFormat="1" ht="38.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="J29" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4">
+    <cfRule type="cellIs" priority="2" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4:J27">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDD6AE8-8F9B-4DFC-A72E-16C1F83D8C08}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added georep1 & 2
</commit_message>
<xml_diff>
--- a/test_sets_UpdateTracking.xlsx
+++ b/test_sets_UpdateTracking.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>Nr</t>
   </si>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1052,9 @@
       <c r="F23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="7"/>
+      <c r="G23" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="H23" s="7"/>
       <c r="J23" s="13"/>
     </row>

</xml_diff>

<commit_message>
added all remaining Test from xlsx
</commit_message>
<xml_diff>
--- a/test_sets_UpdateTracking.xlsx
+++ b/test_sets_UpdateTracking.xlsx
@@ -63,12 +63,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="E19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Stefan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hier hab ich den Punkt vom LocalPlacement geändert bei Placement_Local hab ich ein neues Placement generiert</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Stefan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ich hab hier das alte Placement eine neue Line zugewiesen aber ich hab auch des PointByDistanceExpression anpassen müssen</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Nr</t>
   </si>
@@ -353,27 +401,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -703,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:G20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,10 +762,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -757,7 +798,7 @@
       <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J4" s="12"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -779,7 +820,7 @@
         <v>50</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="J5" s="13"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -801,14 +842,14 @@
         <v>50</v>
       </c>
       <c r="H6" s="7"/>
-      <c r="J6" s="13"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="J7" s="13"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -830,14 +871,14 @@
         <v>50</v>
       </c>
       <c r="H8" s="7"/>
-      <c r="J8" s="13"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="J9" s="13"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -855,7 +896,7 @@
       <c r="I10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J10" s="13"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -871,14 +912,14 @@
       <c r="I11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J11" s="13"/>
+      <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="J12" s="13"/>
+      <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
@@ -897,7 +938,7 @@
         <v>50</v>
       </c>
       <c r="H13" s="7"/>
-      <c r="J13" s="13"/>
+      <c r="J13" s="12"/>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
@@ -916,7 +957,7 @@
         <v>50</v>
       </c>
       <c r="H14" s="7"/>
-      <c r="J14" s="13"/>
+      <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
@@ -934,9 +975,11 @@
       <c r="F15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="H15" s="7"/>
-      <c r="J15" s="13"/>
+      <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
@@ -954,9 +997,11 @@
       <c r="F16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="H16" s="7"/>
-      <c r="J16" s="13"/>
+      <c r="J16" s="12"/>
     </row>
     <row r="17" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
@@ -973,14 +1018,14 @@
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="J17" s="13"/>
+      <c r="J17" s="12"/>
     </row>
     <row r="18" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="J18" s="13"/>
+      <c r="J18" s="12"/>
     </row>
     <row r="19" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
@@ -998,9 +1043,11 @@
       <c r="F19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="7"/>
+      <c r="G19" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="H19" s="7"/>
-      <c r="J19" s="13"/>
+      <c r="J19" s="12"/>
     </row>
     <row r="20" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
@@ -1018,23 +1065,25 @@
       <c r="F20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="7"/>
+      <c r="G20" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="H20" s="7"/>
-      <c r="J20" s="13"/>
+      <c r="J20" s="12"/>
     </row>
     <row r="21" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="J21" s="13"/>
+      <c r="J21" s="12"/>
     </row>
     <row r="22" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-      <c r="J22" s="13"/>
+      <c r="J22" s="12"/>
     </row>
     <row r="23" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
@@ -1056,14 +1105,14 @@
         <v>50</v>
       </c>
       <c r="H23" s="7"/>
-      <c r="J23" s="13"/>
+      <c r="J23" s="12"/>
     </row>
     <row r="24" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="J24" s="13"/>
+      <c r="J24" s="12"/>
     </row>
     <row r="25" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
@@ -1073,42 +1122,42 @@
       <c r="E25" s="3"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
-      <c r="J25" s="13"/>
+      <c r="J25" s="12"/>
     </row>
     <row r="26" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="J26" s="13"/>
+      <c r="J26" s="12"/>
     </row>
     <row r="27" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-      <c r="J27" s="13"/>
+      <c r="J27" s="12"/>
     </row>
     <row r="28" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
-      <c r="J28" s="13"/>
+      <c r="J28" s="12"/>
     </row>
     <row r="29" spans="2:10" s="2" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-      <c r="J29" s="13"/>
+      <c r="J29" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1118,7 +1167,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J27">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated comments in xlsx
</commit_message>
<xml_diff>
--- a/test_sets_UpdateTracking.xlsx
+++ b/test_sets_UpdateTracking.xlsx
@@ -60,6 +60,31 @@
           <t xml:space="preserve">
 Was ist hier mit Subgraphs gemeint? 
 Einfach ein IfcProdukt?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Stefan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Wie soll ich die erstellen. Alle Sweep funktionen die ich sehe basieren auf einem Profil + Axis 
+</t>
         </r>
       </text>
     </comment>
@@ -744,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>